<commit_message>
Added HGT % of genomes assembled at ITM
</commit_message>
<xml_diff>
--- a/STEP4/Percentage_HGT.xlsx
+++ b/STEP4/Percentage_HGT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -611,6 +611,42 @@
   </si>
   <si>
     <t xml:space="preserve">Mycolicibacter_virginiensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_alsense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_angelicum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_diernhoferi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_engbaekii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_europaeum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_fragae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_heraklionense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_iranicum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_paraense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_persicum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_szulgai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_triviale</t>
   </si>
 </sst>
 </file>
@@ -727,15 +763,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A177" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A198" activeCellId="0" sqref="A198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.51"/>
@@ -3648,6 +3684,186 @@
       <c r="D194" s="3" t="n">
         <f aca="false">B194/C194*100</f>
         <v>0.906077348066298</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>5189</v>
+      </c>
+      <c r="D195" s="3" t="n">
+        <f aca="false">B195/C195*100</f>
+        <v>1.9849682019657</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>5415</v>
+      </c>
+      <c r="D196" s="3" t="n">
+        <f aca="false">B196/C196*100</f>
+        <v>3.73037857802401</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="C197" s="0" t="n">
+        <v>5603</v>
+      </c>
+      <c r="D197" s="3" t="n">
+        <f aca="false">B197/C197*100</f>
+        <v>2.51650901302873</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C198" s="0" t="n">
+        <v>4098</v>
+      </c>
+      <c r="D198" s="3" t="n">
+        <f aca="false">B198/C198*100</f>
+        <v>9.27281600780869</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>2674</v>
+      </c>
+      <c r="C199" s="0" t="n">
+        <v>5189</v>
+      </c>
+      <c r="D199" s="3" t="n">
+        <f aca="false">B199/C199*100</f>
+        <v>51.5320871073425</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C200" s="0" t="n">
+        <v>4441</v>
+      </c>
+      <c r="D200" s="3" t="n">
+        <f aca="false">B200/C200*100</f>
+        <v>0.810628236883585</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>418</v>
+      </c>
+      <c r="C201" s="0" t="n">
+        <v>4568</v>
+      </c>
+      <c r="D201" s="3" t="n">
+        <f aca="false">B201/C201*100</f>
+        <v>9.15061295971979</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="C202" s="0" t="n">
+        <v>5965</v>
+      </c>
+      <c r="D202" s="3" t="n">
+        <f aca="false">B202/C202*100</f>
+        <v>2.01173512154233</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="C203" s="0" t="n">
+        <v>5254</v>
+      </c>
+      <c r="D203" s="3" t="n">
+        <f aca="false">B203/C203*100</f>
+        <v>3.90178911305672</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="C204" s="0" t="n">
+        <v>5346</v>
+      </c>
+      <c r="D204" s="3" t="n">
+        <f aca="false">B204/C204*100</f>
+        <v>1.98279087167976</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C205" s="0" t="n">
+        <v>5697</v>
+      </c>
+      <c r="D205" s="3" t="n">
+        <f aca="false">B205/C205*100</f>
+        <v>4.21274354923644</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C206" s="0" t="n">
+        <v>3416</v>
+      </c>
+      <c r="D206" s="3" t="n">
+        <f aca="false">B206/C206*100</f>
+        <v>0.292740046838408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>